<commit_message>
Update RS and code for release 20250218
</commit_message>
<xml_diff>
--- a/FileSyncandWOPI/Docs/MS-ONESTORE/MS-ONESTORE_RequirementSpecification.xlsx
+++ b/FileSyncandWOPI/Docs/MS-ONESTORE/MS-ONESTORE_RequirementSpecification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\TestSuites\Interop-TestSuites-WJP-Commit\FileSyncandWOPI\Docs\MS-ONESTORE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TestSuite\20250218\Interop-TestSuites\FileSyncandWOPI\Docs\MS-ONESTORE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14567F09-12CC-4BD5-ACF2-02878684F739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F836B3B7-B2C9-4802-9172-C03FE11DD4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7053,6 +7053,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7077,21 +7092,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -7100,14 +7100,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="5" tint="0.59996337778862885"/>
+          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59996337778862885"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8811,7 +8811,7 @@
   <dimension ref="A1:O1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D981" sqref="D981"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8854,42 +8854,42 @@
         <v>3</v>
       </c>
       <c r="C3" s="9">
-        <v>13.1</v>
+        <v>13.2</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="10">
-        <v>45608</v>
+        <v>45706</v>
       </c>
       <c r="J3" s="24"/>
     </row>
     <row r="4" spans="1:15" ht="21">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
       <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
       <c r="J5" s="24"/>
       <c r="O5" s="25"/>
     </row>
@@ -8897,96 +8897,96 @@
       <c r="A6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
       <c r="J6" s="24"/>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
       <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
       <c r="J8" s="24"/>
     </row>
     <row r="9" spans="1:15" ht="78.75" customHeight="1">
       <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
       <c r="J9" s="24"/>
     </row>
     <row r="10" spans="1:15" ht="33.75" customHeight="1">
       <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
       <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
       <c r="J11" s="24"/>
     </row>
     <row r="12" spans="1:15">
@@ -8999,12 +8999,12 @@
       <c r="C12" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
       <c r="J12" s="24"/>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1">
@@ -9017,12 +9017,12 @@
       <c r="C13" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
       <c r="J13" s="24"/>
     </row>
     <row r="14" spans="1:15">
@@ -9035,12 +9035,12 @@
       <c r="C14" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
       <c r="J14" s="24"/>
     </row>
     <row r="15" spans="1:15">
@@ -9053,60 +9053,60 @@
       <c r="C15" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
       <c r="J15" s="24"/>
     </row>
     <row r="16" spans="1:15" ht="30" customHeight="1">
       <c r="A16" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
       <c r="J16" s="24"/>
     </row>
     <row r="17" spans="1:10" ht="64.5" customHeight="1">
       <c r="A17" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
       <c r="J17" s="24"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1">
       <c r="A18" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
       <c r="J18" s="24"/>
     </row>
     <row r="19" spans="1:10" ht="30">
@@ -33895,11 +33895,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
     <mergeCell ref="B18:I18"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B9:I9"/>
@@ -33907,34 +33902,39 @@
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="A535:B535 D535:I535">
     <cfRule type="expression" dxfId="197" priority="20">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="196" priority="15">
+    <cfRule type="expression" dxfId="196" priority="17">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="195" priority="15">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="195" priority="16">
+    <cfRule type="expression" dxfId="194" priority="16">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="194" priority="17">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:I28 B29:I46 A29:A534 B47:D241 E47:I534 B242:B243 D242:D243 B244:D244 B245:B247 D245:D247 B248:D248 B249:B251 D249:D251 B252:D252 B253:B255 D253:D255 B256:D272 J257:J260 J262:J265 B273:B274 D273:D274 B275:D276 B277:B278 D277:D278 B279:D376 B377:B382 D377:D382 B383:D429 B430:B439 D430:D439 B440:D457 B458:B459 D458:D459 B460:D485 B486:B487 D486:D487 B488:D491 B492:B494 D492:D494 B495:D534 A536:C538 E536:I538 B540:D542 A540:A618 E540:I618 B543:B546 D543:D546 B547:D558 B559:B564 D559:D564 B565:D568 B569:B573 D569:D573 B574:D577 B578:B580 D578:D580 B581:D617 B618 D618 A619:I632 A633:B635 D633:I635 A636:I638 A639:B639 D639:I639 A640:I644 A645:B646 D645:I646 A647:I649 A650:B650 E650:I650 A651:I683 A684:B694 D684:I694 A695:I702 A703:B703 D703:I703 A704:I731 A732:B733 D732:I733 A734:I742 A743:B745 D743:I745 A746:I746 A747:B751 D747:I751 A752:I752 A753:B757 D753:I757 A758:I759 A760:B760 D760:I760 A761:I763 A764:B768 D764:I768 A769:I769 A770:B771 D770:I771 A772:I792 A793:B793 D793:I793 A794:I813 A814:B814 D814:I814 A815:I816 A817:B818 D817:I818 A819:I827 A828:B832 D828:I832 A833:I860 A861:B861 D861:I861 A862:I865 A866:B866 D866:I866 A867:I867 A868:B868 D868:I868 A869:I899 A900:B900 D900:I900 A901:I905 A906:B907 D906:I907 A908:I909 A910:B913 D910:I913 A914:I926 A927:B927 D927:I927 A928:I928 A929:B929 D929:I929 A930:I931 A932:B932 D932:I932 A933:I965 A966:B966 D966:I966 A967:I989 A990:H990 A991:I998 A999:B999 D999:I999 A1000:I1006">
-    <cfRule type="expression" dxfId="193" priority="429">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    <cfRule type="expression" dxfId="193" priority="383">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="192" priority="385">
+    <cfRule type="expression" dxfId="192" priority="384">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="191" priority="385">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="191" priority="384">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="190" priority="383">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="190" priority="429">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A539:I539">
@@ -33952,17 +33952,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C242:C243">
-    <cfRule type="expression" dxfId="185" priority="320">
+    <cfRule type="expression" dxfId="185" priority="318">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="184" priority="317">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="183" priority="320">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="184" priority="319">
+    <cfRule type="expression" dxfId="182" priority="319">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="183" priority="318">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="182" priority="317">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C245:C247">
@@ -33994,53 +33994,53 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C253:C255">
-    <cfRule type="expression" dxfId="173" priority="302">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="172" priority="301">
+    <cfRule type="expression" dxfId="173" priority="301">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="171" priority="300">
+    <cfRule type="expression" dxfId="172" priority="300">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="170" priority="299">
+    <cfRule type="expression" dxfId="171" priority="299">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="170" priority="302">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C273:C274">
-    <cfRule type="expression" dxfId="169" priority="293">
+    <cfRule type="expression" dxfId="169" priority="294">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="168" priority="293">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="168" priority="296">
+    <cfRule type="expression" dxfId="167" priority="296">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="167" priority="295">
+    <cfRule type="expression" dxfId="166" priority="295">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="166" priority="294">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C277:C278">
-    <cfRule type="expression" dxfId="165" priority="289">
+    <cfRule type="expression" dxfId="165" priority="290">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="164" priority="289">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="164" priority="287">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="163" priority="288">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="290">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    <cfRule type="expression" dxfId="162" priority="287">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C377:C382">
-    <cfRule type="expression" dxfId="161" priority="283">
+    <cfRule type="expression" dxfId="161" priority="284">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="160" priority="283">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="160" priority="284">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="159" priority="282">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
@@ -34050,31 +34050,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C430:C439">
-    <cfRule type="expression" dxfId="157" priority="275">
+    <cfRule type="expression" dxfId="157" priority="278">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="156" priority="276">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="155" priority="275">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="278">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="155" priority="277">
+    <cfRule type="expression" dxfId="154" priority="277">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="154" priority="276">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C458:C459">
-    <cfRule type="expression" dxfId="153" priority="271">
+    <cfRule type="expression" dxfId="153" priority="272">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="152" priority="271">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="272">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    <cfRule type="expression" dxfId="151" priority="270">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="151" priority="269">
+    <cfRule type="expression" dxfId="150" priority="269">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="150" priority="270">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C486:C487">
@@ -34092,45 +34092,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C492:C494">
-    <cfRule type="expression" dxfId="145" priority="260">
+    <cfRule type="expression" dxfId="145" priority="258">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="144" priority="257">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="143" priority="260">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="259">
+    <cfRule type="expression" dxfId="142" priority="259">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="143" priority="258">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C535">
+    <cfRule type="expression" dxfId="141" priority="12">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="140" priority="11">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="139" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="257">
+    <cfRule type="expression" dxfId="138" priority="9">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C535">
-    <cfRule type="expression" dxfId="141" priority="11">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="140" priority="10">
+  <conditionalFormatting sqref="C543:C546">
+    <cfRule type="expression" dxfId="137" priority="252">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="9">
+    <cfRule type="expression" dxfId="136" priority="251">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="12">
+    <cfRule type="expression" dxfId="135" priority="254">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C543:C546">
-    <cfRule type="expression" dxfId="137" priority="254">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="136" priority="253">
+    <cfRule type="expression" dxfId="134" priority="253">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="135" priority="252">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="134" priority="251">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C559:C564">
@@ -34148,17 +34148,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C569:C573">
-    <cfRule type="expression" dxfId="129" priority="239">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="129" priority="242">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="240">
+    <cfRule type="expression" dxfId="128" priority="241">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="127" priority="240">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="241">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="126" priority="242">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    <cfRule type="expression" dxfId="126" priority="239">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C578:C580">
@@ -34176,45 +34176,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C618">
-    <cfRule type="expression" dxfId="121" priority="229">
+    <cfRule type="expression" dxfId="121" priority="230">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="120" priority="229">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="120" priority="227">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="119" priority="228">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="230">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    <cfRule type="expression" dxfId="118" priority="227">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C633:C635">
-    <cfRule type="expression" dxfId="117" priority="223">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="116" priority="224">
+    <cfRule type="expression" dxfId="117" priority="224">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="222">
+    <cfRule type="expression" dxfId="116" priority="222">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="223">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="114" priority="221">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C639">
-    <cfRule type="expression" dxfId="113" priority="218">
+    <cfRule type="expression" dxfId="113" priority="216">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="215">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="111" priority="218">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="216">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="111" priority="217">
+    <cfRule type="expression" dxfId="110" priority="217">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="110" priority="215">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C645:C646">
@@ -34232,45 +34232,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C650">
-    <cfRule type="expression" dxfId="105" priority="206">
+    <cfRule type="expression" dxfId="105" priority="204">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="203">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="103" priority="206">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="205">
+    <cfRule type="expression" dxfId="102" priority="205">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="204">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="102" priority="203">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C684:C694">
-    <cfRule type="expression" dxfId="101" priority="188">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="100" priority="187">
+    <cfRule type="expression" dxfId="101" priority="187">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="186">
+    <cfRule type="expression" dxfId="100" priority="186">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="185">
+    <cfRule type="expression" dxfId="99" priority="185">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="98" priority="188">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C703">
-    <cfRule type="expression" dxfId="97" priority="180">
+    <cfRule type="expression" dxfId="97" priority="182">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="96" priority="181">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="95" priority="180">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="179">
+    <cfRule type="expression" dxfId="94" priority="179">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="95" priority="181">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="94" priority="182">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C732:C733">
@@ -34291,28 +34291,28 @@
     <cfRule type="expression" dxfId="89" priority="164">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="161">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="88" priority="163">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="87" priority="162">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="163">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    <cfRule type="expression" dxfId="86" priority="161">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C747:C751">
-    <cfRule type="expression" dxfId="85" priority="157">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="84" priority="156">
+    <cfRule type="expression" dxfId="85" priority="156">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="155">
+    <cfRule type="expression" dxfId="84" priority="155">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="158">
+    <cfRule type="expression" dxfId="83" priority="158">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="82" priority="157">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C753:C757">
@@ -34330,199 +34330,199 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C760">
-    <cfRule type="expression" dxfId="77" priority="145">
+    <cfRule type="expression" dxfId="77" priority="146">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="145">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="144">
+    <cfRule type="expression" dxfId="75" priority="144">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="143">
+    <cfRule type="expression" dxfId="74" priority="143">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="74" priority="146">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C764:C768">
-    <cfRule type="expression" dxfId="73" priority="125">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="73" priority="128">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="126">
+    <cfRule type="expression" dxfId="72" priority="127">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="71" priority="126">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="128">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="127">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    <cfRule type="expression" dxfId="70" priority="125">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C770:C771">
-    <cfRule type="expression" dxfId="69" priority="113">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="69" priority="116">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="115">
+    <cfRule type="expression" dxfId="68" priority="114">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="115">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="116">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="66" priority="114">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    <cfRule type="expression" dxfId="66" priority="113">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C793">
-    <cfRule type="expression" dxfId="65" priority="108">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    <cfRule type="expression" dxfId="65" priority="110">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="64" priority="109">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="107">
+    <cfRule type="expression" dxfId="63" priority="108">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="107">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="110">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C814">
     <cfRule type="expression" dxfId="61" priority="102">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="104">
+    <cfRule type="expression" dxfId="60" priority="101">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="104">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="59" priority="101">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="58" priority="103">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C817:C818">
-    <cfRule type="expression" dxfId="57" priority="97">
+    <cfRule type="expression" dxfId="57" priority="98">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="97">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="96">
+    <cfRule type="expression" dxfId="55" priority="96">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="95">
+    <cfRule type="expression" dxfId="54" priority="95">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="98">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C828:C832">
-    <cfRule type="expression" dxfId="53" priority="92">
+    <cfRule type="expression" dxfId="53" priority="90">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="89">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="92">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="91">
+    <cfRule type="expression" dxfId="50" priority="91">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="90">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C861">
+    <cfRule type="expression" dxfId="49" priority="86">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="84">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="89">
+    <cfRule type="expression" dxfId="47" priority="83">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="85">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C866">
+    <cfRule type="expression" dxfId="45" priority="80">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="79">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="78">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="77">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C861">
-    <cfRule type="expression" dxfId="49" priority="85">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="48" priority="83">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="47" priority="84">
+  <conditionalFormatting sqref="C868">
+    <cfRule type="expression" dxfId="41" priority="72">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="86">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C866">
-    <cfRule type="expression" dxfId="45" priority="77">
+    <cfRule type="expression" dxfId="40" priority="71">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="78">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="80">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="79">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C868">
-    <cfRule type="expression" dxfId="41" priority="71">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="74">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="39" priority="73">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="72">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    <cfRule type="expression" dxfId="38" priority="74">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C900">
     <cfRule type="expression" dxfId="37" priority="68">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="66">
+    <cfRule type="expression" dxfId="36" priority="67">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="66">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="67">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="34" priority="65">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C906:C907">
-    <cfRule type="expression" dxfId="33" priority="62">
+    <cfRule type="expression" dxfId="33" priority="60">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="59">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="62">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="61">
+    <cfRule type="expression" dxfId="30" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="60">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C910:C913">
+    <cfRule type="expression" dxfId="29" priority="56">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="55">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="59">
+    <cfRule type="expression" dxfId="26" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C910:C913">
-    <cfRule type="expression" dxfId="29" priority="54">
+  <conditionalFormatting sqref="C927">
+    <cfRule type="expression" dxfId="25" priority="50">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="49">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="48">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="53">
+    <cfRule type="expression" dxfId="22" priority="47">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="56">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="55">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C927">
-    <cfRule type="expression" dxfId="25" priority="48">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="47">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="50">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="49">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C929">
@@ -34540,45 +34540,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C932">
-    <cfRule type="expression" dxfId="17" priority="38">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="37">
+    <cfRule type="expression" dxfId="17" priority="37">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="36">
+    <cfRule type="expression" dxfId="16" priority="36">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="35">
+    <cfRule type="expression" dxfId="15" priority="35">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="38">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C966">
-    <cfRule type="expression" dxfId="13" priority="32">
+    <cfRule type="expression" dxfId="13" priority="30">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="29">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="32">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="31">
+    <cfRule type="expression" dxfId="10" priority="31">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="30">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="29">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C999">
-    <cfRule type="expression" dxfId="9" priority="26">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="25">
+    <cfRule type="expression" dxfId="9" priority="25">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="24">
+    <cfRule type="expression" dxfId="8" priority="24">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="23">
+    <cfRule type="expression" dxfId="7" priority="23">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="26">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D536:D538">
@@ -34596,11 +34596,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F1006">
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4">
-      <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">

</xml_diff>

<commit_message>
git revert Update RS and code for MS-ONESTORE release 20250218
</commit_message>
<xml_diff>
--- a/FileSyncandWOPI/Docs/MS-ONESTORE/MS-ONESTORE_RequirementSpecification.xlsx
+++ b/FileSyncandWOPI/Docs/MS-ONESTORE/MS-ONESTORE_RequirementSpecification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TestSuite\20250218\Interop-TestSuites\FileSyncandWOPI\Docs\MS-ONESTORE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\TestSuites\Interop-TestSuites-WJP-Commit\FileSyncandWOPI\Docs\MS-ONESTORE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F836B3B7-B2C9-4802-9172-C03FE11DD4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14567F09-12CC-4BD5-ACF2-02878684F739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7053,21 +7053,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7092,6 +7077,21 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -7100,14 +7100,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="6" tint="0.59996337778862885"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="5" tint="0.59996337778862885"/>
+          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8811,7 +8811,7 @@
   <dimension ref="A1:O1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D981" sqref="D981"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8854,42 +8854,42 @@
         <v>3</v>
       </c>
       <c r="C3" s="9">
-        <v>13.2</v>
+        <v>13.1</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="10">
-        <v>45706</v>
+        <v>45608</v>
       </c>
       <c r="J3" s="24"/>
     </row>
     <row r="4" spans="1:15" ht="21">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
       <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
       <c r="J5" s="24"/>
       <c r="O5" s="25"/>
     </row>
@@ -8897,96 +8897,96 @@
       <c r="A6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
       <c r="J6" s="24"/>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
       <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
       <c r="J8" s="24"/>
     </row>
     <row r="9" spans="1:15" ht="78.75" customHeight="1">
       <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
       <c r="J9" s="24"/>
     </row>
     <row r="10" spans="1:15" ht="33.75" customHeight="1">
       <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
       <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
       <c r="J11" s="24"/>
     </row>
     <row r="12" spans="1:15">
@@ -8999,12 +8999,12 @@
       <c r="C12" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
       <c r="J12" s="24"/>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1">
@@ -9017,12 +9017,12 @@
       <c r="C13" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
       <c r="J13" s="24"/>
     </row>
     <row r="14" spans="1:15">
@@ -9035,12 +9035,12 @@
       <c r="C14" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
       <c r="J14" s="24"/>
     </row>
     <row r="15" spans="1:15">
@@ -9053,60 +9053,60 @@
       <c r="C15" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
       <c r="J15" s="24"/>
     </row>
     <row r="16" spans="1:15" ht="30" customHeight="1">
       <c r="A16" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
       <c r="J16" s="24"/>
     </row>
     <row r="17" spans="1:10" ht="64.5" customHeight="1">
       <c r="A17" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
       <c r="J17" s="24"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1">
       <c r="A18" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
       <c r="J18" s="24"/>
     </row>
     <row r="19" spans="1:10" ht="30">
@@ -33895,6 +33895,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
     <mergeCell ref="B18:I18"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B9:I9"/>
@@ -33902,39 +33907,34 @@
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="A535:B535 D535:I535">
     <cfRule type="expression" dxfId="197" priority="20">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="196" priority="17">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="195" priority="15">
+    <cfRule type="expression" dxfId="196" priority="15">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="194" priority="16">
+    <cfRule type="expression" dxfId="195" priority="16">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="194" priority="17">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:I28 B29:I46 A29:A534 B47:D241 E47:I534 B242:B243 D242:D243 B244:D244 B245:B247 D245:D247 B248:D248 B249:B251 D249:D251 B252:D252 B253:B255 D253:D255 B256:D272 J257:J260 J262:J265 B273:B274 D273:D274 B275:D276 B277:B278 D277:D278 B279:D376 B377:B382 D377:D382 B383:D429 B430:B439 D430:D439 B440:D457 B458:B459 D458:D459 B460:D485 B486:B487 D486:D487 B488:D491 B492:B494 D492:D494 B495:D534 A536:C538 E536:I538 B540:D542 A540:A618 E540:I618 B543:B546 D543:D546 B547:D558 B559:B564 D559:D564 B565:D568 B569:B573 D569:D573 B574:D577 B578:B580 D578:D580 B581:D617 B618 D618 A619:I632 A633:B635 D633:I635 A636:I638 A639:B639 D639:I639 A640:I644 A645:B646 D645:I646 A647:I649 A650:B650 E650:I650 A651:I683 A684:B694 D684:I694 A695:I702 A703:B703 D703:I703 A704:I731 A732:B733 D732:I733 A734:I742 A743:B745 D743:I745 A746:I746 A747:B751 D747:I751 A752:I752 A753:B757 D753:I757 A758:I759 A760:B760 D760:I760 A761:I763 A764:B768 D764:I768 A769:I769 A770:B771 D770:I771 A772:I792 A793:B793 D793:I793 A794:I813 A814:B814 D814:I814 A815:I816 A817:B818 D817:I818 A819:I827 A828:B832 D828:I832 A833:I860 A861:B861 D861:I861 A862:I865 A866:B866 D866:I866 A867:I867 A868:B868 D868:I868 A869:I899 A900:B900 D900:I900 A901:I905 A906:B907 D906:I907 A908:I909 A910:B913 D910:I913 A914:I926 A927:B927 D927:I927 A928:I928 A929:B929 D929:I929 A930:I931 A932:B932 D932:I932 A933:I965 A966:B966 D966:I966 A967:I989 A990:H990 A991:I998 A999:B999 D999:I999 A1000:I1006">
-    <cfRule type="expression" dxfId="193" priority="383">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="193" priority="429">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="192" priority="384">
+    <cfRule type="expression" dxfId="192" priority="385">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="191" priority="384">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="191" priority="385">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="190" priority="429">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    <cfRule type="expression" dxfId="190" priority="383">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A539:I539">
@@ -33952,17 +33952,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C242:C243">
-    <cfRule type="expression" dxfId="185" priority="318">
+    <cfRule type="expression" dxfId="185" priority="320">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="184" priority="319">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="183" priority="318">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="184" priority="317">
+    <cfRule type="expression" dxfId="182" priority="317">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="183" priority="320">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="182" priority="319">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C245:C247">
@@ -33994,53 +33994,53 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C253:C255">
-    <cfRule type="expression" dxfId="173" priority="301">
+    <cfRule type="expression" dxfId="173" priority="302">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="172" priority="301">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="172" priority="300">
+    <cfRule type="expression" dxfId="171" priority="300">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="171" priority="299">
+    <cfRule type="expression" dxfId="170" priority="299">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="170" priority="302">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C273:C274">
-    <cfRule type="expression" dxfId="169" priority="294">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="168" priority="293">
+    <cfRule type="expression" dxfId="169" priority="293">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="167" priority="296">
+    <cfRule type="expression" dxfId="168" priority="296">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="295">
+    <cfRule type="expression" dxfId="167" priority="295">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="166" priority="294">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C277:C278">
-    <cfRule type="expression" dxfId="165" priority="290">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    <cfRule type="expression" dxfId="165" priority="289">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="164" priority="289">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    <cfRule type="expression" dxfId="164" priority="287">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="163" priority="288">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="287">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="162" priority="290">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C377:C382">
-    <cfRule type="expression" dxfId="161" priority="284">
+    <cfRule type="expression" dxfId="161" priority="283">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="160" priority="284">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="160" priority="283">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="159" priority="282">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
@@ -34050,31 +34050,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C430:C439">
-    <cfRule type="expression" dxfId="157" priority="278">
+    <cfRule type="expression" dxfId="157" priority="275">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="156" priority="278">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="276">
+    <cfRule type="expression" dxfId="155" priority="277">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="154" priority="276">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="155" priority="275">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="154" priority="277">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C458:C459">
-    <cfRule type="expression" dxfId="153" priority="272">
+    <cfRule type="expression" dxfId="153" priority="271">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="152" priority="272">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="271">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    <cfRule type="expression" dxfId="151" priority="269">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="151" priority="270">
+    <cfRule type="expression" dxfId="150" priority="270">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="150" priority="269">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C486:C487">
@@ -34092,45 +34092,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C492:C494">
-    <cfRule type="expression" dxfId="145" priority="258">
+    <cfRule type="expression" dxfId="145" priority="260">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="144" priority="259">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="143" priority="258">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="257">
+    <cfRule type="expression" dxfId="142" priority="257">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="143" priority="260">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="142" priority="259">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C535">
-    <cfRule type="expression" dxfId="141" priority="12">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="140" priority="11">
+    <cfRule type="expression" dxfId="141" priority="11">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="10">
+    <cfRule type="expression" dxfId="140" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="9">
+    <cfRule type="expression" dxfId="139" priority="9">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="138" priority="12">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C543:C546">
-    <cfRule type="expression" dxfId="137" priority="252">
+    <cfRule type="expression" dxfId="137" priority="254">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="136" priority="253">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="135" priority="252">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="251">
+    <cfRule type="expression" dxfId="134" priority="251">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="135" priority="254">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="134" priority="253">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C559:C564">
@@ -34148,17 +34148,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C569:C573">
-    <cfRule type="expression" dxfId="129" priority="242">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    <cfRule type="expression" dxfId="129" priority="239">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="241">
+    <cfRule type="expression" dxfId="128" priority="240">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="127" priority="241">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="240">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="126" priority="239">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="126" priority="242">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C578:C580">
@@ -34176,45 +34176,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C618">
-    <cfRule type="expression" dxfId="121" priority="230">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    <cfRule type="expression" dxfId="121" priority="229">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="229">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    <cfRule type="expression" dxfId="120" priority="227">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="119" priority="228">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="227">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="118" priority="230">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C633:C635">
-    <cfRule type="expression" dxfId="117" priority="224">
+    <cfRule type="expression" dxfId="117" priority="223">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="116" priority="224">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="222">
+    <cfRule type="expression" dxfId="115" priority="222">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="115" priority="223">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="114" priority="221">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C639">
-    <cfRule type="expression" dxfId="113" priority="216">
+    <cfRule type="expression" dxfId="113" priority="218">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="216">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="215">
+    <cfRule type="expression" dxfId="111" priority="217">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="110" priority="215">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="111" priority="218">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="110" priority="217">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C645:C646">
@@ -34232,45 +34232,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C650">
-    <cfRule type="expression" dxfId="105" priority="204">
+    <cfRule type="expression" dxfId="105" priority="206">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="205">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="103" priority="204">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="203">
+    <cfRule type="expression" dxfId="102" priority="203">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="206">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="102" priority="205">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C684:C694">
-    <cfRule type="expression" dxfId="101" priority="187">
+    <cfRule type="expression" dxfId="101" priority="188">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="100" priority="187">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="186">
+    <cfRule type="expression" dxfId="99" priority="186">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="185">
+    <cfRule type="expression" dxfId="98" priority="185">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="98" priority="188">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C703">
-    <cfRule type="expression" dxfId="97" priority="182">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    <cfRule type="expression" dxfId="97" priority="180">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="181">
+    <cfRule type="expression" dxfId="96" priority="179">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="95" priority="181">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="180">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="94" priority="179">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="94" priority="182">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C732:C733">
@@ -34291,28 +34291,28 @@
     <cfRule type="expression" dxfId="89" priority="164">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="163">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    <cfRule type="expression" dxfId="88" priority="161">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="87" priority="162">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="161">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="86" priority="163">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C747:C751">
-    <cfRule type="expression" dxfId="85" priority="156">
+    <cfRule type="expression" dxfId="85" priority="157">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="84" priority="156">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="155">
+    <cfRule type="expression" dxfId="83" priority="155">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="158">
+    <cfRule type="expression" dxfId="82" priority="158">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="82" priority="157">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C753:C757">
@@ -34330,199 +34330,199 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C760">
-    <cfRule type="expression" dxfId="77" priority="146">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="76" priority="145">
+    <cfRule type="expression" dxfId="77" priority="145">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="144">
+    <cfRule type="expression" dxfId="76" priority="144">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="143">
+    <cfRule type="expression" dxfId="75" priority="143">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="74" priority="146">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C764:C768">
-    <cfRule type="expression" dxfId="73" priority="128">
+    <cfRule type="expression" dxfId="73" priority="125">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="126">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="71" priority="128">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="127">
+    <cfRule type="expression" dxfId="70" priority="127">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="71" priority="126">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="125">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C770:C771">
-    <cfRule type="expression" dxfId="69" priority="116">
+    <cfRule type="expression" dxfId="69" priority="113">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="115">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="116">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="114">
+    <cfRule type="expression" dxfId="66" priority="114">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="115">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="66" priority="113">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C793">
-    <cfRule type="expression" dxfId="65" priority="110">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    <cfRule type="expression" dxfId="65" priority="108">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="64" priority="109">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="108">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    <cfRule type="expression" dxfId="63" priority="107">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="107">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    <cfRule type="expression" dxfId="62" priority="110">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C814">
     <cfRule type="expression" dxfId="61" priority="102">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="101">
+    <cfRule type="expression" dxfId="60" priority="104">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="101">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="59" priority="104">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="58" priority="103">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C817:C818">
-    <cfRule type="expression" dxfId="57" priority="98">
+    <cfRule type="expression" dxfId="57" priority="97">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="96">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="95">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="98">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="97">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C828:C832">
+    <cfRule type="expression" dxfId="53" priority="92">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="91">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="96">
+    <cfRule type="expression" dxfId="51" priority="90">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="95">
+    <cfRule type="expression" dxfId="50" priority="89">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C828:C832">
-    <cfRule type="expression" dxfId="53" priority="90">
+  <conditionalFormatting sqref="C861">
+    <cfRule type="expression" dxfId="49" priority="85">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="83">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="47" priority="84">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="89">
+    <cfRule type="expression" dxfId="46" priority="86">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C866">
+    <cfRule type="expression" dxfId="45" priority="77">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="92">
+    <cfRule type="expression" dxfId="44" priority="78">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="80">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="91">
+    <cfRule type="expression" dxfId="42" priority="79">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C861">
-    <cfRule type="expression" dxfId="49" priority="86">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="48" priority="84">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="47" priority="83">
+  <conditionalFormatting sqref="C868">
+    <cfRule type="expression" dxfId="41" priority="71">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="85">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C866">
-    <cfRule type="expression" dxfId="45" priority="80">
+    <cfRule type="expression" dxfId="40" priority="74">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="79">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="78">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="77">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C868">
-    <cfRule type="expression" dxfId="41" priority="72">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="71">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="39" priority="73">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="74">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    <cfRule type="expression" dxfId="38" priority="72">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C900">
     <cfRule type="expression" dxfId="37" priority="68">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="67">
+    <cfRule type="expression" dxfId="36" priority="66">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="67">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="66">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="34" priority="65">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C906:C907">
-    <cfRule type="expression" dxfId="33" priority="60">
+    <cfRule type="expression" dxfId="33" priority="62">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="61">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="60">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="59">
+    <cfRule type="expression" dxfId="30" priority="59">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="62">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C910:C913">
+    <cfRule type="expression" dxfId="29" priority="54">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="53">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="56">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="61">
+    <cfRule type="expression" dxfId="26" priority="55">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C910:C913">
-    <cfRule type="expression" dxfId="29" priority="56">
+  <conditionalFormatting sqref="C927">
+    <cfRule type="expression" dxfId="25" priority="48">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="47">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="50">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="55">
+    <cfRule type="expression" dxfId="22" priority="49">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="54">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="53">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C927">
-    <cfRule type="expression" dxfId="25" priority="50">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="49">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="48">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="47">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C929">
@@ -34540,45 +34540,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C932">
-    <cfRule type="expression" dxfId="17" priority="37">
+    <cfRule type="expression" dxfId="17" priority="38">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="37">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="36">
+    <cfRule type="expression" dxfId="15" priority="36">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="35">
+    <cfRule type="expression" dxfId="14" priority="35">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="38">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C966">
-    <cfRule type="expression" dxfId="13" priority="30">
+    <cfRule type="expression" dxfId="13" priority="32">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="31">
+      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="30">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="29">
+    <cfRule type="expression" dxfId="10" priority="29">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="32">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="31">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C999">
-    <cfRule type="expression" dxfId="9" priority="25">
+    <cfRule type="expression" dxfId="9" priority="26">
+      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="25">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="24">
+    <cfRule type="expression" dxfId="7" priority="24">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="23">
+    <cfRule type="expression" dxfId="6" priority="23">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="26">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D536:D538">
@@ -34596,11 +34596,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F1006">
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="1" priority="5">
+      <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="5">
-      <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">

</xml_diff>